<commit_message>
round 16 predictions 2021
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Collingwood_stats.xlsx
+++ b/django_AFL_ML/Data/Collingwood_stats.xlsx
@@ -4,13 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
 </workbook>
 </file>
 
@@ -59,34 +59,34 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -380,19 +380,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IJ102"/>
+  <dimension ref="A1:IK102"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="HZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="IN24" activeCellId="0" sqref="IN24"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="HZ1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="IN24" activeCellId="0" pane="topLeft" sqref="IN24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col width="8.529999999999999" customWidth="1" style="2" min="1" max="1016"/>
-    <col width="9.140000000000001" customWidth="1" style="2" min="1017" max="1025"/>
+    <col customWidth="1" max="1016" min="1" style="2" width="8.529999999999999"/>
+    <col customWidth="1" max="1025" min="1017" style="2" width="9.140000000000001"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="1" s="3">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Match_ID</t>
@@ -1124,11 +1124,14 @@
       <c r="II1" s="2" t="n">
         <v>10429</v>
       </c>
-      <c r="IJ1" t="n">
+      <c r="IJ1" s="2" t="n">
         <v>10432</v>
       </c>
+      <c r="IK1" t="n">
+        <v>10446</v>
+      </c>
     </row>
-    <row r="2" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="2" s="3">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Year</t>
@@ -1860,11 +1863,14 @@
       <c r="II2" s="2" t="n">
         <v>2021</v>
       </c>
-      <c r="IJ2" t="n">
+      <c r="IJ2" s="2" t="n">
         <v>2021</v>
       </c>
+      <c r="IK2" t="n">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="3" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="3" s="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Round</t>
@@ -2596,11 +2602,14 @@
       <c r="II3" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="IJ3" t="n">
+      <c r="IJ3" s="2" t="n">
         <v>13</v>
       </c>
+      <c r="IK3" t="n">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="4" s="3">
       <c r="A4" s="2" t="inlineStr">
         <is>
           <t>H/A?</t>
@@ -3332,11 +3341,14 @@
       <c r="II4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IJ4" t="n">
+      <c r="IJ4" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="IK4" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="5" s="3">
       <c r="A5" s="2" t="inlineStr">
         <is>
           <t>H/A Win?</t>
@@ -4068,11 +4080,14 @@
       <c r="II5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IJ5" t="n">
+      <c r="IJ5" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="IK5" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="6" s="3">
       <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Points For</t>
@@ -4804,11 +4819,14 @@
       <c r="II6" s="2" t="n">
         <v>78</v>
       </c>
-      <c r="IJ6" t="n">
+      <c r="IJ6" s="2" t="n">
         <v>80</v>
       </c>
+      <c r="IK6" t="n">
+        <v>79</v>
+      </c>
     </row>
-    <row r="7" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="7" s="3">
       <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Points Against</t>
@@ -5540,11 +5558,14 @@
       <c r="II7" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="IJ7" t="n">
+      <c r="IJ7" s="2" t="n">
         <v>63</v>
       </c>
+      <c r="IK7" t="n">
+        <v>91</v>
+      </c>
     </row>
-    <row r="8" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="8" s="3">
       <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Margin</t>
@@ -6276,11 +6297,14 @@
       <c r="II8" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="IJ8" t="n">
+      <c r="IJ8" s="2" t="n">
         <v>17</v>
       </c>
+      <c r="IK8" t="n">
+        <v>-12</v>
+      </c>
     </row>
-    <row r="9" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="9" s="3">
       <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Team Won? (1=W, 0=L)</t>
@@ -7012,11 +7036,14 @@
       <c r="II9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IJ9" t="n">
+      <c r="IJ9" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="IK9" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="10" s="3">
       <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Team_against_ID</t>
@@ -7748,11 +7775,14 @@
       <c r="II10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IJ10" t="n">
+      <c r="IJ10" s="2" t="n">
         <v>11</v>
       </c>
+      <c r="IK10" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row r="11" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="11" s="3">
       <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Kicks</t>
@@ -8484,11 +8514,14 @@
       <c r="II11" s="2" t="n">
         <v>225</v>
       </c>
-      <c r="IJ11" t="n">
+      <c r="IJ11" s="2" t="n">
         <v>237</v>
       </c>
+      <c r="IK11" t="n">
+        <v>238</v>
+      </c>
     </row>
-    <row r="12" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="12" s="3">
       <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Handballs</t>
@@ -9220,11 +9253,14 @@
       <c r="II12" s="2" t="n">
         <v>109</v>
       </c>
-      <c r="IJ12" t="n">
+      <c r="IJ12" s="2" t="n">
         <v>158</v>
       </c>
+      <c r="IK12" t="n">
+        <v>162</v>
+      </c>
     </row>
-    <row r="13" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="13" s="3">
       <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Disposals</t>
@@ -9956,11 +9992,14 @@
       <c r="II13" s="2" t="n">
         <v>334</v>
       </c>
-      <c r="IJ13" t="n">
+      <c r="IJ13" s="2" t="n">
         <v>395</v>
       </c>
+      <c r="IK13" t="n">
+        <v>400</v>
+      </c>
     </row>
-    <row r="14" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="14" s="3">
       <c r="A14" s="2" t="inlineStr">
         <is>
           <t>Kick to HB Ratio</t>
@@ -10692,11 +10731,14 @@
       <c r="II14" s="2" t="n">
         <v>2.06</v>
       </c>
-      <c r="IJ14" t="n">
+      <c r="IJ14" s="2" t="n">
         <v>1.5</v>
       </c>
+      <c r="IK14" t="n">
+        <v>1.47</v>
+      </c>
     </row>
-    <row r="15" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="15" s="3">
       <c r="A15" s="2" t="inlineStr">
         <is>
           <t>Marks</t>
@@ -11428,11 +11470,14 @@
       <c r="II15" s="2" t="n">
         <v>115</v>
       </c>
-      <c r="IJ15" t="n">
+      <c r="IJ15" s="2" t="n">
         <v>124</v>
       </c>
+      <c r="IK15" t="n">
+        <v>129</v>
+      </c>
     </row>
-    <row r="16" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="16" s="3">
       <c r="A16" s="2" t="inlineStr">
         <is>
           <t>Tackles</t>
@@ -12164,11 +12209,14 @@
       <c r="II16" s="2" t="n">
         <v>76</v>
       </c>
-      <c r="IJ16" t="n">
+      <c r="IJ16" s="2" t="n">
         <v>53</v>
       </c>
+      <c r="IK16" t="n">
+        <v>56</v>
+      </c>
     </row>
-    <row r="17" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="17" s="3">
       <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Hitouts</t>
@@ -12900,11 +12948,14 @@
       <c r="II17" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="IJ17" t="n">
+      <c r="IJ17" s="2" t="n">
         <v>33</v>
       </c>
+      <c r="IK17" t="n">
+        <v>29</v>
+      </c>
     </row>
-    <row r="18" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="18" s="3">
       <c r="A18" s="2" t="inlineStr">
         <is>
           <t>Frees For</t>
@@ -13636,11 +13687,14 @@
       <c r="II18" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="IJ18" t="n">
+      <c r="IJ18" s="2" t="n">
         <v>17</v>
       </c>
+      <c r="IK18" t="n">
+        <v>21</v>
+      </c>
     </row>
-    <row r="19" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="19" s="3">
       <c r="A19" s="2" t="inlineStr">
         <is>
           <t>Frees Against</t>
@@ -14372,11 +14426,14 @@
       <c r="II19" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="IJ19" t="n">
+      <c r="IJ19" s="2" t="n">
         <v>28</v>
       </c>
+      <c r="IK19" t="n">
+        <v>17</v>
+      </c>
     </row>
-    <row r="20" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="20" s="3">
       <c r="A20" s="2" t="inlineStr">
         <is>
           <t>Goals Kicked</t>
@@ -15108,11 +15165,14 @@
       <c r="II20" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="IJ20" t="n">
+      <c r="IJ20" s="2" t="n">
         <v>11</v>
       </c>
+      <c r="IK20" t="n">
+        <v>12</v>
+      </c>
     </row>
-    <row r="21" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="21" s="3">
       <c r="A21" s="2" t="inlineStr">
         <is>
           <t>Goal Assists1</t>
@@ -15844,11 +15904,14 @@
       <c r="II21" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="IJ21" t="n">
+      <c r="IJ21" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="IK21" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row r="22" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="22" s="3">
       <c r="A22" s="2" t="inlineStr">
         <is>
           <t>Behinds Kicked</t>
@@ -16580,11 +16643,14 @@
       <c r="II22" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="IJ22" t="n">
+      <c r="IJ22" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="IK22" t="n">
+        <v>7</v>
+      </c>
     </row>
-    <row r="23" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="23" s="3">
       <c r="A23" s="2" t="inlineStr">
         <is>
           <t>Rushed Behinds</t>
@@ -17316,11 +17382,14 @@
       <c r="II23" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IJ23" t="n">
+      <c r="IJ23" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="IK23" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="24" s="3">
       <c r="A24" s="2" t="inlineStr">
         <is>
           <t>Scoring Shots</t>
@@ -18052,11 +18121,14 @@
       <c r="II24" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="IJ24" t="n">
+      <c r="IJ24" s="2" t="n">
         <v>25</v>
       </c>
+      <c r="IK24" t="n">
+        <v>19</v>
+      </c>
     </row>
-    <row r="25" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="25" s="3">
       <c r="A25" s="2" t="inlineStr">
         <is>
           <t>Conversion %</t>
@@ -18788,11 +18860,14 @@
       <c r="II25" s="2" t="n">
         <v>66.7</v>
       </c>
-      <c r="IJ25" t="n">
+      <c r="IJ25" s="2" t="n">
         <v>44</v>
       </c>
+      <c r="IK25" t="n">
+        <v>63.2</v>
+      </c>
     </row>
-    <row r="26" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="26" s="3">
       <c r="A26" s="2" t="inlineStr">
         <is>
           <t>Disposals Per Goal</t>
@@ -19524,11 +19599,14 @@
       <c r="II26" s="2" t="n">
         <v>27.83</v>
       </c>
-      <c r="IJ26" t="n">
+      <c r="IJ26" s="2" t="n">
         <v>35.91</v>
       </c>
+      <c r="IK26" t="n">
+        <v>33.33</v>
+      </c>
     </row>
-    <row r="27" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="27" s="3">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Disposals Per Scoring Shot</t>
@@ -20260,11 +20338,14 @@
       <c r="II27" s="2" t="n">
         <v>18.56</v>
       </c>
-      <c r="IJ27" t="n">
+      <c r="IJ27" s="2" t="n">
         <v>15.8</v>
       </c>
+      <c r="IK27" t="n">
+        <v>21.05</v>
+      </c>
     </row>
-    <row r="28" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="28" s="3">
       <c r="A28" s="2" t="inlineStr">
         <is>
           <t>Clearances1</t>
@@ -20996,11 +21077,14 @@
       <c r="II28" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="IJ28" t="n">
+      <c r="IJ28" s="2" t="n">
         <v>34</v>
       </c>
+      <c r="IK28" t="n">
+        <v>23</v>
+      </c>
     </row>
-    <row r="29" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="29" s="3">
       <c r="A29" s="2" t="inlineStr">
         <is>
           <t>Clangers1</t>
@@ -21732,11 +21816,14 @@
       <c r="II29" s="2" t="n">
         <v>54</v>
       </c>
-      <c r="IJ29" t="n">
+      <c r="IJ29" s="2" t="n">
         <v>73</v>
       </c>
+      <c r="IK29" t="n">
+        <v>54</v>
+      </c>
     </row>
-    <row r="30" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="30" s="3">
       <c r="A30" s="2" t="inlineStr">
         <is>
           <t>Rebound 50s1</t>
@@ -22468,11 +22555,14 @@
       <c r="II30" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="IJ30" t="n">
+      <c r="IJ30" s="2" t="n">
         <v>43</v>
       </c>
+      <c r="IK30" t="n">
+        <v>36</v>
+      </c>
     </row>
-    <row r="31" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="31" s="3">
       <c r="A31" s="2" t="inlineStr">
         <is>
           <t>Inside 50s</t>
@@ -23204,11 +23294,14 @@
       <c r="II31" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="IJ31" t="n">
+      <c r="IJ31" s="2" t="n">
         <v>47</v>
       </c>
+      <c r="IK31" t="n">
+        <v>47</v>
+      </c>
     </row>
-    <row r="32" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="32" s="3">
       <c r="A32" s="2" t="inlineStr">
         <is>
           <t>In50s Per Scoring Shot</t>
@@ -23940,11 +24033,14 @@
       <c r="II32" s="2" t="n">
         <v>2.44</v>
       </c>
-      <c r="IJ32" t="n">
+      <c r="IJ32" s="2" t="n">
         <v>1.88</v>
       </c>
+      <c r="IK32" t="n">
+        <v>2.47</v>
+      </c>
     </row>
-    <row r="33" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="33" s="3">
       <c r="A33" s="2" t="inlineStr">
         <is>
           <t>In50s Per Goal</t>
@@ -24676,11 +24772,14 @@
       <c r="II33" s="2" t="n">
         <v>3.67</v>
       </c>
-      <c r="IJ33" t="n">
+      <c r="IJ33" s="2" t="n">
         <v>4.27</v>
       </c>
+      <c r="IK33" t="n">
+        <v>3.92</v>
+      </c>
     </row>
-    <row r="34" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="34" s="3">
       <c r="A34" s="2" t="inlineStr">
         <is>
           <t>% In50s Score</t>
@@ -25412,11 +25511,14 @@
       <c r="II34" s="2" t="n">
         <v>38.6</v>
       </c>
-      <c r="IJ34" t="n">
+      <c r="IJ34" s="2" t="n">
         <v>40.4</v>
       </c>
+      <c r="IK34" t="n">
+        <v>40.4</v>
+      </c>
     </row>
-    <row r="35" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="35" s="3">
       <c r="A35" s="2" t="inlineStr">
         <is>
           <t>% In50s Goal</t>
@@ -26148,11 +26250,14 @@
       <c r="II35" s="2" t="n">
         <v>27.3</v>
       </c>
-      <c r="IJ35" t="n">
+      <c r="IJ35" s="2" t="n">
         <v>23.4</v>
       </c>
+      <c r="IK35" t="n">
+        <v>25.5</v>
+      </c>
     </row>
-    <row r="36" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="36" s="3">
       <c r="A36" s="2" t="inlineStr">
         <is>
           <t>Height</t>
@@ -26884,11 +26989,14 @@
       <c r="II36" s="2" t="n">
         <v>188.1</v>
       </c>
-      <c r="IJ36" t="n">
+      <c r="IJ36" s="2" t="n">
         <v>188.3</v>
       </c>
+      <c r="IK36" t="n">
+        <v>188.3</v>
+      </c>
     </row>
-    <row r="37" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="37" s="3">
       <c r="A37" s="2" t="inlineStr">
         <is>
           <t>Weight</t>
@@ -27620,11 +27728,14 @@
       <c r="II37" s="2" t="n">
         <v>86.90000000000001</v>
       </c>
-      <c r="IJ37" t="n">
+      <c r="IJ37" s="2" t="n">
         <v>86.8</v>
       </c>
+      <c r="IK37" t="n">
+        <v>86.5</v>
+      </c>
     </row>
-    <row r="38" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="38" s="3">
       <c r="A38" s="2" t="inlineStr">
         <is>
           <t>Age</t>
@@ -28356,11 +28467,14 @@
       <c r="II38" s="2" t="n">
         <v>25.41</v>
       </c>
-      <c r="IJ38" t="n">
+      <c r="IJ38" s="2" t="n">
         <v>25.66</v>
       </c>
+      <c r="IK38" t="n">
+        <v>26.33</v>
+      </c>
     </row>
-    <row r="39" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="39" s="3">
       <c r="A39" s="2" t="inlineStr">
         <is>
           <t>Av Games</t>
@@ -29092,11 +29206,14 @@
       <c r="II39" s="2" t="n">
         <v>86.8</v>
       </c>
-      <c r="IJ39" t="n">
+      <c r="IJ39" s="2" t="n">
         <v>94.7</v>
       </c>
+      <c r="IK39" t="n">
+        <v>105.8</v>
+      </c>
     </row>
-    <row r="40" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="40" s="3">
       <c r="A40" s="2" t="inlineStr">
         <is>
           <t>&lt;50 Games</t>
@@ -29828,11 +29945,14 @@
       <c r="II40" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="IJ40" t="n">
+      <c r="IJ40" s="2" t="n">
         <v>11</v>
       </c>
+      <c r="IK40" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row r="41" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="41" s="3">
       <c r="A41" s="2" t="inlineStr">
         <is>
           <t>50-99 Games</t>
@@ -30564,11 +30684,14 @@
       <c r="II41" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="IJ41" t="n">
+      <c r="IJ41" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="IK41" t="n">
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="42" s="3">
       <c r="A42" s="2" t="inlineStr">
         <is>
           <t>100-149 Games</t>
@@ -31300,11 +31423,14 @@
       <c r="II42" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="IJ42" t="n">
+      <c r="IJ42" s="2" t="n">
         <v>6</v>
       </c>
+      <c r="IK42" t="n">
+        <v>3</v>
+      </c>
     </row>
-    <row r="43" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="43" s="3">
       <c r="A43" s="2" t="inlineStr">
         <is>
           <t>&gt;150 Games</t>
@@ -32036,11 +32162,14 @@
       <c r="II43" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="IJ43" t="n">
+      <c r="IJ43" s="2" t="n">
         <v>5</v>
       </c>
+      <c r="IK43" t="n">
+        <v>8</v>
+      </c>
     </row>
-    <row r="44" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="44" s="3">
       <c r="A44" s="2" t="inlineStr">
         <is>
           <t>Contested Poss</t>
@@ -32772,11 +32901,14 @@
       <c r="II44" s="2" t="n">
         <v>122</v>
       </c>
-      <c r="IJ44" t="n">
+      <c r="IJ44" s="2" t="n">
         <v>126</v>
       </c>
+      <c r="IK44" t="n">
+        <v>124</v>
+      </c>
     </row>
-    <row r="45" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="45" s="3">
       <c r="A45" s="2" t="inlineStr">
         <is>
           <t>Uncontested Poss</t>
@@ -33508,11 +33640,14 @@
       <c r="II45" s="2" t="n">
         <v>206</v>
       </c>
-      <c r="IJ45" t="n">
+      <c r="IJ45" s="2" t="n">
         <v>257</v>
       </c>
+      <c r="IK45" t="n">
+        <v>270</v>
+      </c>
     </row>
-    <row r="46" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="46" s="3">
       <c r="A46" s="2" t="inlineStr">
         <is>
           <t>Effective Disposals</t>
@@ -34244,11 +34379,14 @@
       <c r="II46" s="2" t="n">
         <v>252</v>
       </c>
-      <c r="IJ46" t="n">
+      <c r="IJ46" s="2" t="n">
         <v>290</v>
       </c>
+      <c r="IK46" t="n">
+        <v>310</v>
+      </c>
     </row>
-    <row r="47" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="47" s="3">
       <c r="A47" s="2" t="inlineStr">
         <is>
           <t>Disposal Efficiency</t>
@@ -34980,11 +35118,14 @@
       <c r="II47" s="2" t="n">
         <v>75.40000000000001</v>
       </c>
-      <c r="IJ47" t="n">
+      <c r="IJ47" s="2" t="n">
         <v>73.40000000000001</v>
       </c>
+      <c r="IK47" t="n">
+        <v>77.5</v>
+      </c>
     </row>
-    <row r="48" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="48" s="3">
       <c r="A48" s="2" t="inlineStr">
         <is>
           <t>Clangers2</t>
@@ -35716,11 +35857,14 @@
       <c r="II48" s="2" t="n">
         <v>54</v>
       </c>
-      <c r="IJ48" t="n">
+      <c r="IJ48" s="2" t="n">
         <v>73</v>
       </c>
+      <c r="IK48" t="n">
+        <v>54</v>
+      </c>
     </row>
-    <row r="49" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="49" s="3">
       <c r="A49" s="2" t="inlineStr">
         <is>
           <t>Contested Marks</t>
@@ -36452,11 +36596,14 @@
       <c r="II49" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="IJ49" t="n">
+      <c r="IJ49" s="2" t="n">
         <v>14</v>
       </c>
+      <c r="IK49" t="n">
+        <v>16</v>
+      </c>
     </row>
-    <row r="50" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="50" s="3">
       <c r="A50" s="2" t="inlineStr">
         <is>
           <t>Marks Inside 50</t>
@@ -37188,11 +37335,14 @@
       <c r="II50" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="IJ50" t="n">
+      <c r="IJ50" s="2" t="n">
         <v>18</v>
       </c>
+      <c r="IK50" t="n">
+        <v>14</v>
+      </c>
     </row>
-    <row r="51" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="51" s="3">
       <c r="A51" s="2" t="inlineStr">
         <is>
           <t>Clearances2</t>
@@ -37924,11 +38074,14 @@
       <c r="II51" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="IJ51" t="n">
+      <c r="IJ51" s="2" t="n">
         <v>34</v>
       </c>
+      <c r="IK51" t="n">
+        <v>23</v>
+      </c>
     </row>
-    <row r="52" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="52" s="3">
       <c r="A52" s="2" t="inlineStr">
         <is>
           <t>Rebound 50s2</t>
@@ -38660,11 +38813,14 @@
       <c r="II52" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="IJ52" t="n">
+      <c r="IJ52" s="2" t="n">
         <v>43</v>
       </c>
+      <c r="IK52" t="n">
+        <v>36</v>
+      </c>
     </row>
-    <row r="53" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="53" s="3">
       <c r="A53" s="2" t="inlineStr">
         <is>
           <t>1%ers</t>
@@ -39396,11 +39552,14 @@
       <c r="II53" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="IJ53" t="n">
+      <c r="IJ53" s="2" t="n">
         <v>52</v>
       </c>
+      <c r="IK53" t="n">
+        <v>36</v>
+      </c>
     </row>
-    <row r="54" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="54" s="3">
       <c r="A54" s="2" t="inlineStr">
         <is>
           <t>Bounces</t>
@@ -40132,11 +40291,14 @@
       <c r="II54" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IJ54" t="n">
+      <c r="IJ54" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="IK54" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row r="55" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="55" s="3">
       <c r="A55" s="2" t="inlineStr">
         <is>
           <t>Goals Assists2</t>
@@ -40868,11 +41030,14 @@
       <c r="II55" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="IJ55" t="n">
+      <c r="IJ55" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="IK55" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row r="56" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="56" s="3">
       <c r="A56" s="2" t="inlineStr">
         <is>
           <t>Goal Assist %</t>
@@ -41604,11 +41769,14 @@
       <c r="II56" s="2" t="n">
         <v>83.3</v>
       </c>
-      <c r="IJ56" t="n">
+      <c r="IJ56" s="2" t="n">
         <v>72.7</v>
       </c>
+      <c r="IK56" t="n">
+        <v>75</v>
+      </c>
     </row>
-    <row r="57" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="57" s="3">
       <c r="A57" s="2" t="inlineStr">
         <is>
           <t>Kicks (O)</t>
@@ -42340,11 +42508,14 @@
       <c r="II57" s="2" t="n">
         <v>202</v>
       </c>
-      <c r="IJ57" t="n">
+      <c r="IJ57" s="2" t="n">
         <v>203</v>
       </c>
+      <c r="IK57" t="n">
+        <v>198</v>
+      </c>
     </row>
-    <row r="58" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="58" s="3">
       <c r="A58" s="2" t="inlineStr">
         <is>
           <t>Handballs (O)</t>
@@ -43076,11 +43247,14 @@
       <c r="II58" s="2" t="n">
         <v>155</v>
       </c>
-      <c r="IJ58" t="n">
+      <c r="IJ58" s="2" t="n">
         <v>154</v>
       </c>
+      <c r="IK58" t="n">
+        <v>148</v>
+      </c>
     </row>
-    <row r="59" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="59" s="3">
       <c r="A59" s="2" t="inlineStr">
         <is>
           <t>Disposals (O)</t>
@@ -43812,11 +43986,14 @@
       <c r="II59" s="2" t="n">
         <v>357</v>
       </c>
-      <c r="IJ59" t="n">
+      <c r="IJ59" s="2" t="n">
         <v>357</v>
       </c>
+      <c r="IK59" t="n">
+        <v>346</v>
+      </c>
     </row>
-    <row r="60" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="60" s="3">
       <c r="A60" s="2" t="inlineStr">
         <is>
           <t>Kick to HB Ratio (O)</t>
@@ -44548,11 +44725,14 @@
       <c r="II60" s="2" t="n">
         <v>1.3</v>
       </c>
-      <c r="IJ60" t="n">
+      <c r="IJ60" s="2" t="n">
         <v>1.32</v>
       </c>
+      <c r="IK60" t="n">
+        <v>1.34</v>
+      </c>
     </row>
-    <row r="61" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="61" s="3">
       <c r="A61" s="2" t="inlineStr">
         <is>
           <t>Marks (O)</t>
@@ -45284,11 +45464,14 @@
       <c r="II61" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="IJ61" t="n">
+      <c r="IJ61" s="2" t="n">
         <v>97</v>
       </c>
+      <c r="IK61" t="n">
+        <v>85</v>
+      </c>
     </row>
-    <row r="62" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="62" s="3">
       <c r="A62" s="2" t="inlineStr">
         <is>
           <t>Tackles(O)</t>
@@ -46020,11 +46203,14 @@
       <c r="II62" s="2" t="n">
         <v>52</v>
       </c>
-      <c r="IJ62" t="n">
+      <c r="IJ62" s="2" t="n">
         <v>43</v>
       </c>
+      <c r="IK62" t="n">
+        <v>34</v>
+      </c>
     </row>
-    <row r="63" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="63" s="3">
       <c r="A63" s="2" t="inlineStr">
         <is>
           <t>Hitouts(O)</t>
@@ -46756,11 +46942,14 @@
       <c r="II63" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="IJ63" t="n">
+      <c r="IJ63" s="2" t="n">
         <v>26</v>
       </c>
+      <c r="IK63" t="n">
+        <v>20</v>
+      </c>
     </row>
-    <row r="64" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="64" s="3">
       <c r="A64" s="2" t="inlineStr">
         <is>
           <t>Frees For(O)</t>
@@ -47492,11 +47681,14 @@
       <c r="II64" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="IJ64" t="n">
+      <c r="IJ64" s="2" t="n">
         <v>28</v>
       </c>
+      <c r="IK64" t="n">
+        <v>17</v>
+      </c>
     </row>
-    <row r="65" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="65" s="3">
       <c r="A65" s="2" t="inlineStr">
         <is>
           <t>Frees Against(O)</t>
@@ -48228,11 +48420,14 @@
       <c r="II65" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="IJ65" t="n">
+      <c r="IJ65" s="2" t="n">
         <v>17</v>
       </c>
+      <c r="IK65" t="n">
+        <v>21</v>
+      </c>
     </row>
-    <row r="66" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="66" s="3">
       <c r="A66" s="2" t="inlineStr">
         <is>
           <t>Goals Kicked(O)</t>
@@ -48964,11 +49159,14 @@
       <c r="II66" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="IJ66" t="n">
+      <c r="IJ66" s="2" t="n">
         <v>9</v>
       </c>
+      <c r="IK66" t="n">
+        <v>14</v>
+      </c>
     </row>
-    <row r="67" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="67" s="3">
       <c r="A67" s="2" t="inlineStr">
         <is>
           <t>Goal Assists1(O)</t>
@@ -49700,11 +49898,14 @@
       <c r="II67" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="IJ67" t="n">
+      <c r="IJ67" s="2" t="n">
         <v>5</v>
       </c>
+      <c r="IK67" t="n">
+        <v>11</v>
+      </c>
     </row>
-    <row r="68" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="68" s="3">
       <c r="A68" s="2" t="inlineStr">
         <is>
           <t>Behinds Kicked(O)</t>
@@ -50436,11 +50637,14 @@
       <c r="II68" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="IJ68" t="n">
+      <c r="IJ68" s="2" t="n">
         <v>7</v>
       </c>
+      <c r="IK68" t="n">
+        <v>7</v>
+      </c>
     </row>
-    <row r="69" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="69" s="3">
       <c r="A69" s="2" t="inlineStr">
         <is>
           <t>Rushed Behinds(O)</t>
@@ -51172,11 +51376,14 @@
       <c r="II69" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="IJ69" t="n">
+      <c r="IJ69" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="IK69" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="70" s="3">
       <c r="A70" s="2" t="inlineStr">
         <is>
           <t>Scoring Shots(O)</t>
@@ -51908,11 +52115,14 @@
       <c r="II70" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="IJ70" t="n">
+      <c r="IJ70" s="2" t="n">
         <v>18</v>
       </c>
+      <c r="IK70" t="n">
+        <v>21</v>
+      </c>
     </row>
-    <row r="71" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="71" s="3">
       <c r="A71" s="2" t="inlineStr">
         <is>
           <t>Conversion %(O)</t>
@@ -52644,11 +52854,14 @@
       <c r="II71" s="2" t="n">
         <v>43.5</v>
       </c>
-      <c r="IJ71" t="n">
+      <c r="IJ71" s="2" t="n">
         <v>50</v>
       </c>
+      <c r="IK71" t="n">
+        <v>66.7</v>
+      </c>
     </row>
-    <row r="72" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="72" s="3">
       <c r="A72" s="2" t="inlineStr">
         <is>
           <t>Disposals Per Goal(O)</t>
@@ -53380,11 +53593,14 @@
       <c r="II72" s="2" t="n">
         <v>35.7</v>
       </c>
-      <c r="IJ72" t="n">
+      <c r="IJ72" s="2" t="n">
         <v>39.67</v>
       </c>
+      <c r="IK72" t="n">
+        <v>24.71</v>
+      </c>
     </row>
-    <row r="73" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="73" s="3">
       <c r="A73" s="2" t="inlineStr">
         <is>
           <t>Disposals Per Scoring Shot(O)</t>
@@ -54116,11 +54332,14 @@
       <c r="II73" s="2" t="n">
         <v>15.52</v>
       </c>
-      <c r="IJ73" t="n">
+      <c r="IJ73" s="2" t="n">
         <v>19.83</v>
       </c>
+      <c r="IK73" t="n">
+        <v>16.48</v>
+      </c>
     </row>
-    <row r="74" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="74" s="3">
       <c r="A74" s="2" t="inlineStr">
         <is>
           <t>Clearances1(O)</t>
@@ -54852,11 +55071,14 @@
       <c r="II74" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="IJ74" t="n">
+      <c r="IJ74" s="2" t="n">
         <v>24</v>
       </c>
+      <c r="IK74" t="n">
+        <v>34</v>
+      </c>
     </row>
-    <row r="75" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="75" s="3">
       <c r="A75" s="2" t="inlineStr">
         <is>
           <t>Clangers1(O)</t>
@@ -55588,11 +55810,14 @@
       <c r="II75" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="IJ75" t="n">
+      <c r="IJ75" s="2" t="n">
         <v>51</v>
       </c>
+      <c r="IK75" t="n">
+        <v>52</v>
+      </c>
     </row>
-    <row r="76" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="76" s="3">
       <c r="A76" s="2" t="inlineStr">
         <is>
           <t>Rebound 50s1(O)</t>
@@ -56324,11 +56549,14 @@
       <c r="II76" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="IJ76" t="n">
+      <c r="IJ76" s="2" t="n">
         <v>36</v>
       </c>
+      <c r="IK76" t="n">
+        <v>34</v>
+      </c>
     </row>
-    <row r="77" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="77" s="3">
       <c r="A77" s="2" t="inlineStr">
         <is>
           <t>Inside 50s(O)</t>
@@ -57060,11 +57288,14 @@
       <c r="II77" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="IJ77" t="n">
+      <c r="IJ77" s="2" t="n">
         <v>53</v>
       </c>
+      <c r="IK77" t="n">
+        <v>51</v>
+      </c>
     </row>
-    <row r="78" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="78" s="3">
       <c r="A78" s="2" t="inlineStr">
         <is>
           <t>In50s Per Scoring Shot(O)</t>
@@ -57796,11 +58027,14 @@
       <c r="II78" s="2" t="n">
         <v>2.17</v>
       </c>
-      <c r="IJ78" t="n">
+      <c r="IJ78" s="2" t="n">
         <v>2.94</v>
       </c>
+      <c r="IK78" t="n">
+        <v>2.43</v>
+      </c>
     </row>
-    <row r="79" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="79" s="3">
       <c r="A79" s="2" t="inlineStr">
         <is>
           <t>In50s Per Goal(O)</t>
@@ -58532,11 +58766,14 @@
       <c r="II79" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="IJ79" t="n">
+      <c r="IJ79" s="2" t="n">
         <v>5.89</v>
       </c>
+      <c r="IK79" t="n">
+        <v>3.64</v>
+      </c>
     </row>
-    <row r="80" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="80" s="3">
       <c r="A80" s="2" t="inlineStr">
         <is>
           <t>% In50s Score(O)</t>
@@ -59268,11 +59505,14 @@
       <c r="II80" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="IJ80" t="n">
+      <c r="IJ80" s="2" t="n">
         <v>30.2</v>
       </c>
+      <c r="IK80" t="n">
+        <v>41.2</v>
+      </c>
     </row>
-    <row r="81" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="81" s="3">
       <c r="A81" s="2" t="inlineStr">
         <is>
           <t>% In50s Goal(O)</t>
@@ -60004,11 +60244,14 @@
       <c r="II81" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="IJ81" t="n">
+      <c r="IJ81" s="2" t="n">
         <v>17</v>
       </c>
+      <c r="IK81" t="n">
+        <v>27.5</v>
+      </c>
     </row>
-    <row r="82" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="82" s="3">
       <c r="A82" s="2" t="inlineStr">
         <is>
           <t>Height(O)</t>
@@ -60740,11 +60983,14 @@
       <c r="II82" s="2" t="n">
         <v>186.8</v>
       </c>
-      <c r="IJ82" t="n">
+      <c r="IJ82" s="2" t="n">
         <v>187.9</v>
       </c>
+      <c r="IK82" t="n">
+        <v>187</v>
+      </c>
     </row>
-    <row r="83" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="83" s="3">
       <c r="A83" s="2" t="inlineStr">
         <is>
           <t>Weight(O)</t>
@@ -61476,11 +61722,14 @@
       <c r="II83" s="2" t="n">
         <v>84.09999999999999</v>
       </c>
-      <c r="IJ83" t="n">
+      <c r="IJ83" s="2" t="n">
         <v>86.2</v>
       </c>
+      <c r="IK83" t="n">
+        <v>87.2</v>
+      </c>
     </row>
-    <row r="84" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="84" s="3">
       <c r="A84" s="2" t="inlineStr">
         <is>
           <t>Age(O)</t>
@@ -62212,11 +62461,14 @@
       <c r="II84" s="2" t="n">
         <v>24.49</v>
       </c>
-      <c r="IJ84" t="n">
+      <c r="IJ84" s="2" t="n">
         <v>24.58</v>
       </c>
+      <c r="IK84" t="n">
+        <v>24.91</v>
+      </c>
     </row>
-    <row r="85" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="85" s="3">
       <c r="A85" s="2" t="inlineStr">
         <is>
           <t>Av Games(O)</t>
@@ -62948,11 +63200,14 @@
       <c r="II85" s="2" t="n">
         <v>73.7</v>
       </c>
-      <c r="IJ85" t="n">
+      <c r="IJ85" s="2" t="n">
         <v>85.5</v>
       </c>
+      <c r="IK85" t="n">
+        <v>79.3</v>
+      </c>
     </row>
-    <row r="86" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="86" s="3">
       <c r="A86" s="2" t="inlineStr">
         <is>
           <t>&lt;50 Games(O)</t>
@@ -63684,11 +63939,14 @@
       <c r="II86" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="IJ86" t="n">
+      <c r="IJ86" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="IK86" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row r="87" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="87" s="3">
       <c r="A87" s="2" t="inlineStr">
         <is>
           <t>50-99 Games(O)</t>
@@ -64420,11 +64678,14 @@
       <c r="II87" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="IJ87" t="n">
+      <c r="IJ87" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="IK87" t="n">
+        <v>8</v>
+      </c>
     </row>
-    <row r="88" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="88" s="3">
       <c r="A88" s="2" t="inlineStr">
         <is>
           <t>100-149 Games(O)</t>
@@ -65156,11 +65417,14 @@
       <c r="II88" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="IJ88" t="n">
+      <c r="IJ88" s="2" t="n">
         <v>7</v>
       </c>
+      <c r="IK88" t="n">
+        <v>4</v>
+      </c>
     </row>
-    <row r="89" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="89" s="3">
       <c r="A89" s="2" t="inlineStr">
         <is>
           <t>&gt;150 Games(O)</t>
@@ -65892,11 +66156,14 @@
       <c r="II89" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="IJ89" t="n">
+      <c r="IJ89" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="IK89" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row r="90" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="90" s="3">
       <c r="A90" s="2" t="inlineStr">
         <is>
           <t>Contested Poss(O)</t>
@@ -66628,11 +66895,14 @@
       <c r="II90" s="2" t="n">
         <v>142</v>
       </c>
-      <c r="IJ90" t="n">
+      <c r="IJ90" s="2" t="n">
         <v>125</v>
       </c>
+      <c r="IK90" t="n">
+        <v>120</v>
+      </c>
     </row>
-    <row r="91" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="91" s="3">
       <c r="A91" s="2" t="inlineStr">
         <is>
           <t>Uncontested Poss(O)</t>
@@ -67364,11 +67634,14 @@
       <c r="II91" s="2" t="n">
         <v>211</v>
       </c>
-      <c r="IJ91" t="n">
+      <c r="IJ91" s="2" t="n">
         <v>223</v>
       </c>
+      <c r="IK91" t="n">
+        <v>218</v>
+      </c>
     </row>
-    <row r="92" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="92" s="3">
       <c r="A92" s="2" t="inlineStr">
         <is>
           <t>Effective Disposals(O)</t>
@@ -68100,11 +68373,14 @@
       <c r="II92" s="2" t="n">
         <v>258</v>
       </c>
-      <c r="IJ92" t="n">
+      <c r="IJ92" s="2" t="n">
         <v>267</v>
       </c>
+      <c r="IK92" t="n">
+        <v>268</v>
+      </c>
     </row>
-    <row r="93" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="93" s="3">
       <c r="A93" s="2" t="inlineStr">
         <is>
           <t>Disposal Efficiency(O)</t>
@@ -68836,11 +69112,14 @@
       <c r="II93" s="2" t="n">
         <v>72.3</v>
       </c>
-      <c r="IJ93" t="n">
+      <c r="IJ93" s="2" t="n">
         <v>74.8</v>
       </c>
+      <c r="IK93" t="n">
+        <v>77.5</v>
+      </c>
     </row>
-    <row r="94" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="94" s="3">
       <c r="A94" s="2" t="inlineStr">
         <is>
           <t>Clangers2(O)</t>
@@ -69572,11 +69851,14 @@
       <c r="II94" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="IJ94" t="n">
+      <c r="IJ94" s="2" t="n">
         <v>51</v>
       </c>
+      <c r="IK94" t="n">
+        <v>52</v>
+      </c>
     </row>
-    <row r="95" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="95" s="3">
       <c r="A95" s="2" t="inlineStr">
         <is>
           <t>Contested Marks(O)</t>
@@ -70308,11 +70590,14 @@
       <c r="II95" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="IJ95" t="n">
+      <c r="IJ95" s="2" t="n">
         <v>14</v>
       </c>
+      <c r="IK95" t="n">
+        <v>8</v>
+      </c>
     </row>
-    <row r="96" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="96" s="3">
       <c r="A96" s="2" t="inlineStr">
         <is>
           <t>Marks Inside 50(O)</t>
@@ -71044,11 +71329,14 @@
       <c r="II96" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="IJ96" t="n">
+      <c r="IJ96" s="2" t="n">
         <v>9</v>
       </c>
+      <c r="IK96" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row r="97" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="97" s="3">
       <c r="A97" s="2" t="inlineStr">
         <is>
           <t>Clearances2(O)</t>
@@ -71780,11 +72068,14 @@
       <c r="II97" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="IJ97" t="n">
+      <c r="IJ97" s="2" t="n">
         <v>24</v>
       </c>
+      <c r="IK97" t="n">
+        <v>34</v>
+      </c>
     </row>
-    <row r="98" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="98" s="3">
       <c r="A98" s="2" t="inlineStr">
         <is>
           <t>Rebound 50s2(O)</t>
@@ -72516,11 +72807,14 @@
       <c r="II98" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="IJ98" t="n">
+      <c r="IJ98" s="2" t="n">
         <v>36</v>
       </c>
+      <c r="IK98" t="n">
+        <v>34</v>
+      </c>
     </row>
-    <row r="99" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="99" s="3">
       <c r="A99" s="2" t="inlineStr">
         <is>
           <t>1%ers(O)</t>
@@ -73252,11 +73546,14 @@
       <c r="II99" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="IJ99" t="n">
+      <c r="IJ99" s="2" t="n">
         <v>46</v>
       </c>
+      <c r="IK99" t="n">
+        <v>54</v>
+      </c>
     </row>
-    <row r="100" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="100" s="3">
       <c r="A100" s="2" t="inlineStr">
         <is>
           <t>Bounces(O)</t>
@@ -73988,11 +74285,14 @@
       <c r="II100" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="IJ100" t="n">
+      <c r="IJ100" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="IK100" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row r="101" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="101" s="3">
       <c r="A101" s="2" t="inlineStr">
         <is>
           <t>Goals Assists2(O)</t>
@@ -74724,11 +75024,14 @@
       <c r="II101" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="IJ101" t="n">
+      <c r="IJ101" s="2" t="n">
         <v>5</v>
       </c>
+      <c r="IK101" t="n">
+        <v>11</v>
+      </c>
     </row>
-    <row r="102" ht="13.8" customHeight="1" s="3">
+    <row customHeight="1" ht="13.8" r="102" s="3">
       <c r="A102" s="2" t="inlineStr">
         <is>
           <t>Goal Assist %(O)</t>
@@ -75460,13 +75763,16 @@
       <c r="II102" s="2" t="n">
         <v>90</v>
       </c>
-      <c r="IJ102" t="n">
+      <c r="IJ102" s="2" t="n">
         <v>55.6</v>
+      </c>
+      <c r="IK102" t="n">
+        <v>78.59999999999999</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed getting upcoming games, added requirements txt
</commit_message>
<xml_diff>
--- a/django_AFL_ML/Data/Collingwood_stats.xlsx
+++ b/django_AFL_ML/Data/Collingwood_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:JX102"/>
+  <dimension ref="A1:JZ102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="HZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="IN24" activeCellId="0" sqref="IN24"/>
@@ -1312,8 +1312,14 @@
       <c r="JW1" s="2" t="n">
         <v>10747</v>
       </c>
-      <c r="JX1" t="n">
+      <c r="JX1" s="2" t="n">
         <v>10747</v>
+      </c>
+      <c r="JY1" s="2" t="n">
+        <v>10749</v>
+      </c>
+      <c r="JZ1" t="n">
+        <v>10749</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="3">
@@ -2168,7 +2174,13 @@
       <c r="JW2" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="JX2" t="n">
+      <c r="JX2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JY2" s="2" t="n">
+        <v>2022</v>
+      </c>
+      <c r="JZ2" t="n">
         <v>2022</v>
       </c>
     </row>
@@ -3024,8 +3036,14 @@
       <c r="JW3" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="JX3" t="n">
+      <c r="JX3" s="2" t="n">
         <v>26</v>
+      </c>
+      <c r="JY3" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="JZ3" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="3">
@@ -3880,8 +3898,14 @@
       <c r="JW4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="JX4" t="n">
+      <c r="JX4" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="JY4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="JZ4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.8" customHeight="1" s="3">
@@ -4736,7 +4760,13 @@
       <c r="JW5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="JX5" t="n">
+      <c r="JX5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JY5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JZ5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5592,8 +5622,14 @@
       <c r="JW6" s="2" t="n">
         <v>79</v>
       </c>
-      <c r="JX6" t="n">
+      <c r="JX6" s="2" t="n">
         <v>79</v>
+      </c>
+      <c r="JY6" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="JZ6" t="n">
+        <v>94</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="3">
@@ -6448,8 +6484,14 @@
       <c r="JW7" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="JX7" t="n">
+      <c r="JX7" s="2" t="n">
         <v>59</v>
+      </c>
+      <c r="JY7" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="JZ7" t="n">
+        <v>95</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="3">
@@ -7304,8 +7346,14 @@
       <c r="JW8" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="JX8" t="n">
+      <c r="JX8" s="2" t="n">
         <v>20</v>
+      </c>
+      <c r="JY8" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="JZ8" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="3">
@@ -8160,8 +8208,14 @@
       <c r="JW9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="JX9" t="n">
+      <c r="JX9" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="JY9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="JZ9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="3">
@@ -9016,8 +9070,14 @@
       <c r="JW10" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JX10" t="n">
+      <c r="JX10" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="JY10" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="JZ10" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="3">
@@ -9872,8 +9932,14 @@
       <c r="JW11" s="2" t="n">
         <v>205</v>
       </c>
-      <c r="JX11" t="n">
+      <c r="JX11" s="2" t="n">
         <v>205</v>
+      </c>
+      <c r="JY11" s="2" t="n">
+        <v>193</v>
+      </c>
+      <c r="JZ11" t="n">
+        <v>193</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="3">
@@ -10728,8 +10794,14 @@
       <c r="JW12" s="2" t="n">
         <v>126</v>
       </c>
-      <c r="JX12" t="n">
+      <c r="JX12" s="2" t="n">
         <v>126</v>
+      </c>
+      <c r="JY12" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="JZ12" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="3">
@@ -11584,8 +11656,14 @@
       <c r="JW13" s="2" t="n">
         <v>331</v>
       </c>
-      <c r="JX13" t="n">
+      <c r="JX13" s="2" t="n">
         <v>331</v>
+      </c>
+      <c r="JY13" s="2" t="n">
+        <v>303</v>
+      </c>
+      <c r="JZ13" t="n">
+        <v>303</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="3">
@@ -12440,8 +12518,14 @@
       <c r="JW14" s="2" t="n">
         <v>1.63</v>
       </c>
-      <c r="JX14" t="n">
+      <c r="JX14" s="2" t="n">
         <v>1.63</v>
+      </c>
+      <c r="JY14" s="2" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="JZ14" t="n">
+        <v>1.75</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="3">
@@ -13296,8 +13380,14 @@
       <c r="JW15" s="2" t="n">
         <v>87</v>
       </c>
-      <c r="JX15" t="n">
+      <c r="JX15" s="2" t="n">
         <v>87</v>
+      </c>
+      <c r="JY15" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="JZ15" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="3">
@@ -14152,8 +14242,14 @@
       <c r="JW16" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="JX16" t="n">
+      <c r="JX16" s="2" t="n">
         <v>58</v>
+      </c>
+      <c r="JY16" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="JZ16" t="n">
+        <v>80</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="3">
@@ -15008,8 +15104,14 @@
       <c r="JW17" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="JX17" t="n">
+      <c r="JX17" s="2" t="n">
         <v>33</v>
+      </c>
+      <c r="JY17" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="JZ17" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="3">
@@ -15864,8 +15966,14 @@
       <c r="JW18" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="JX18" t="n">
+      <c r="JX18" s="2" t="n">
         <v>19</v>
+      </c>
+      <c r="JY18" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="JZ18" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="3">
@@ -16720,8 +16828,14 @@
       <c r="JW19" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="JX19" t="n">
+      <c r="JX19" s="2" t="n">
         <v>24</v>
+      </c>
+      <c r="JY19" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="JZ19" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="3">
@@ -17576,8 +17690,14 @@
       <c r="JW20" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="JX20" t="n">
+      <c r="JX20" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="JY20" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JZ20" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="3">
@@ -18432,8 +18552,14 @@
       <c r="JW21" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JX21" t="n">
+      <c r="JX21" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="JY21" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JZ21" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="3">
@@ -19288,8 +19414,14 @@
       <c r="JW22" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="JX22" t="n">
+      <c r="JX22" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="JY22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JZ22" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="3">
@@ -20144,8 +20276,14 @@
       <c r="JW23" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="JX23" t="n">
+      <c r="JX23" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="JY23" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JZ23" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" s="3">
@@ -21000,7 +21138,13 @@
       <c r="JW24" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="JX24" t="n">
+      <c r="JX24" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="JY24" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="JZ24" t="n">
         <v>24</v>
       </c>
     </row>
@@ -21856,8 +22000,14 @@
       <c r="JW25" s="2" t="n">
         <v>45.8</v>
       </c>
-      <c r="JX25" t="n">
+      <c r="JX25" s="2" t="n">
         <v>45.8</v>
+      </c>
+      <c r="JY25" s="2" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="JZ25" t="n">
+        <v>58.3</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="3">
@@ -22712,8 +22862,14 @@
       <c r="JW26" s="2" t="n">
         <v>30.09</v>
       </c>
-      <c r="JX26" t="n">
+      <c r="JX26" s="2" t="n">
         <v>30.09</v>
+      </c>
+      <c r="JY26" s="2" t="n">
+        <v>21.64</v>
+      </c>
+      <c r="JZ26" t="n">
+        <v>21.64</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="3">
@@ -23568,8 +23724,14 @@
       <c r="JW27" s="2" t="n">
         <v>13.79</v>
       </c>
-      <c r="JX27" t="n">
+      <c r="JX27" s="2" t="n">
         <v>13.79</v>
+      </c>
+      <c r="JY27" s="2" t="n">
+        <v>12.62</v>
+      </c>
+      <c r="JZ27" t="n">
+        <v>12.62</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="3">
@@ -24424,8 +24586,14 @@
       <c r="JW28" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="JX28" t="n">
+      <c r="JX28" s="2" t="n">
         <v>33</v>
+      </c>
+      <c r="JY28" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="JZ28" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="3">
@@ -25280,8 +25448,14 @@
       <c r="JW29" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="JX29" t="n">
+      <c r="JX29" s="2" t="n">
         <v>66</v>
+      </c>
+      <c r="JY29" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JZ29" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="3">
@@ -26136,8 +26310,14 @@
       <c r="JW30" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="JX30" t="n">
+      <c r="JX30" s="2" t="n">
         <v>32</v>
+      </c>
+      <c r="JY30" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="JZ30" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="3">
@@ -26992,8 +27172,14 @@
       <c r="JW31" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="JX31" t="n">
+      <c r="JX31" s="2" t="n">
         <v>56</v>
+      </c>
+      <c r="JY31" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="JZ31" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="3">
@@ -27848,8 +28034,14 @@
       <c r="JW32" s="2" t="n">
         <v>2.33</v>
       </c>
-      <c r="JX32" t="n">
+      <c r="JX32" s="2" t="n">
         <v>2.33</v>
+      </c>
+      <c r="JY32" s="2" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="JZ32" t="n">
+        <v>2.58</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="3">
@@ -28704,8 +28896,14 @@
       <c r="JW33" s="2" t="n">
         <v>5.09</v>
       </c>
-      <c r="JX33" t="n">
+      <c r="JX33" s="2" t="n">
         <v>5.09</v>
+      </c>
+      <c r="JY33" s="2" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="JZ33" t="n">
+        <v>4.43</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="3">
@@ -29560,8 +29758,14 @@
       <c r="JW34" s="2" t="n">
         <v>39.3</v>
       </c>
-      <c r="JX34" t="n">
+      <c r="JX34" s="2" t="n">
         <v>39.3</v>
+      </c>
+      <c r="JY34" s="2" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="JZ34" t="n">
+        <v>33.9</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="3">
@@ -30416,8 +30620,14 @@
       <c r="JW35" s="2" t="n">
         <v>19.6</v>
       </c>
-      <c r="JX35" t="n">
+      <c r="JX35" s="2" t="n">
         <v>19.6</v>
+      </c>
+      <c r="JY35" s="2" t="n">
+        <v>22.6</v>
+      </c>
+      <c r="JZ35" t="n">
+        <v>22.6</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="3">
@@ -31272,8 +31482,14 @@
       <c r="JW36" s="2" t="n">
         <v>188.9</v>
       </c>
-      <c r="JX36" t="n">
+      <c r="JX36" s="2" t="n">
         <v>188.9</v>
+      </c>
+      <c r="JY36" s="2" t="n">
+        <v>189.2</v>
+      </c>
+      <c r="JZ36" t="n">
+        <v>189.2</v>
       </c>
     </row>
     <row r="37" ht="13.8" customHeight="1" s="3">
@@ -32128,7 +32344,13 @@
       <c r="JW37" s="2" t="n">
         <v>86.40000000000001</v>
       </c>
-      <c r="JX37" t="n">
+      <c r="JX37" s="2" t="n">
+        <v>86.40000000000001</v>
+      </c>
+      <c r="JY37" s="2" t="n">
+        <v>86.40000000000001</v>
+      </c>
+      <c r="JZ37" t="n">
         <v>86.40000000000001</v>
       </c>
     </row>
@@ -32984,8 +33206,14 @@
       <c r="JW38" s="2" t="n">
         <v>26.16</v>
       </c>
-      <c r="JX38" t="n">
+      <c r="JX38" s="2" t="n">
         <v>26.16</v>
+      </c>
+      <c r="JY38" s="2" t="n">
+        <v>26.24</v>
+      </c>
+      <c r="JZ38" t="n">
+        <v>26.24</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="3">
@@ -33840,8 +34068,14 @@
       <c r="JW39" s="2" t="n">
         <v>108.6</v>
       </c>
-      <c r="JX39" t="n">
+      <c r="JX39" s="2" t="n">
         <v>108.6</v>
+      </c>
+      <c r="JY39" s="2" t="n">
+        <v>109.6</v>
+      </c>
+      <c r="JZ39" t="n">
+        <v>109.6</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="3">
@@ -34696,7 +34930,13 @@
       <c r="JW40" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JX40" t="n">
+      <c r="JX40" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JY40" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JZ40" t="n">
         <v>7</v>
       </c>
     </row>
@@ -35552,7 +35792,13 @@
       <c r="JW41" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JX41" t="n">
+      <c r="JX41" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JY41" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JZ41" t="n">
         <v>6</v>
       </c>
     </row>
@@ -36408,7 +36654,13 @@
       <c r="JW42" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="JX42" t="n">
+      <c r="JX42" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JY42" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="JZ42" t="n">
         <v>3</v>
       </c>
     </row>
@@ -37264,7 +37516,13 @@
       <c r="JW43" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JX43" t="n">
+      <c r="JX43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JY43" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JZ43" t="n">
         <v>7</v>
       </c>
     </row>
@@ -38120,8 +38378,14 @@
       <c r="JW44" s="2" t="n">
         <v>142</v>
       </c>
-      <c r="JX44" t="n">
+      <c r="JX44" s="2" t="n">
         <v>142</v>
+      </c>
+      <c r="JY44" s="2" t="n">
+        <v>134</v>
+      </c>
+      <c r="JZ44" t="n">
+        <v>134</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="3">
@@ -38976,8 +39240,14 @@
       <c r="JW45" s="2" t="n">
         <v>197</v>
       </c>
-      <c r="JX45" t="n">
+      <c r="JX45" s="2" t="n">
         <v>197</v>
+      </c>
+      <c r="JY45" s="2" t="n">
+        <v>157</v>
+      </c>
+      <c r="JZ45" t="n">
+        <v>157</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="3">
@@ -39832,8 +40102,14 @@
       <c r="JW46" s="2" t="n">
         <v>239</v>
       </c>
-      <c r="JX46" t="n">
+      <c r="JX46" s="2" t="n">
         <v>239</v>
+      </c>
+      <c r="JY46" s="2" t="n">
+        <v>201</v>
+      </c>
+      <c r="JZ46" t="n">
+        <v>201</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="3">
@@ -40688,8 +40964,14 @@
       <c r="JW47" s="2" t="n">
         <v>72.2</v>
       </c>
-      <c r="JX47" t="n">
+      <c r="JX47" s="2" t="n">
         <v>72.2</v>
+      </c>
+      <c r="JY47" s="2" t="n">
+        <v>66.3</v>
+      </c>
+      <c r="JZ47" t="n">
+        <v>66.3</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="3">
@@ -41544,8 +41826,14 @@
       <c r="JW48" s="2" t="n">
         <v>66</v>
       </c>
-      <c r="JX48" t="n">
+      <c r="JX48" s="2" t="n">
         <v>66</v>
+      </c>
+      <c r="JY48" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JZ48" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="3">
@@ -42400,8 +42688,14 @@
       <c r="JW49" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JX49" t="n">
+      <c r="JX49" s="2" t="n">
         <v>9</v>
+      </c>
+      <c r="JY49" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="JZ49" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="50" ht="13.8" customHeight="1" s="3">
@@ -43256,8 +43550,14 @@
       <c r="JW50" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="JX50" t="n">
+      <c r="JX50" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="JY50" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="JZ50" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="3">
@@ -44112,8 +44412,14 @@
       <c r="JW51" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="JX51" t="n">
+      <c r="JX51" s="2" t="n">
         <v>33</v>
+      </c>
+      <c r="JY51" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="JZ51" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="3">
@@ -44968,8 +45274,14 @@
       <c r="JW52" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="JX52" t="n">
+      <c r="JX52" s="2" t="n">
         <v>32</v>
+      </c>
+      <c r="JY52" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="JZ52" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="3">
@@ -45824,8 +46136,14 @@
       <c r="JW53" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="JX53" t="n">
+      <c r="JX53" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="JY53" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="JZ53" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="3">
@@ -46680,8 +46998,14 @@
       <c r="JW54" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="JX54" t="n">
+      <c r="JX54" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="JY54" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JZ54" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="3">
@@ -47536,8 +47860,14 @@
       <c r="JW55" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JX55" t="n">
+      <c r="JX55" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="JY55" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JZ55" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="3">
@@ -48392,8 +48722,14 @@
       <c r="JW56" s="2" t="n">
         <v>54.5</v>
       </c>
-      <c r="JX56" t="n">
+      <c r="JX56" s="2" t="n">
         <v>54.5</v>
+      </c>
+      <c r="JY56" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="JZ56" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="3">
@@ -49248,8 +49584,14 @@
       <c r="JW57" s="2" t="n">
         <v>216</v>
       </c>
-      <c r="JX57" t="n">
+      <c r="JX57" s="2" t="n">
         <v>216</v>
+      </c>
+      <c r="JY57" s="2" t="n">
+        <v>217</v>
+      </c>
+      <c r="JZ57" t="n">
+        <v>217</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="3">
@@ -50104,8 +50446,14 @@
       <c r="JW58" s="2" t="n">
         <v>148</v>
       </c>
-      <c r="JX58" t="n">
+      <c r="JX58" s="2" t="n">
         <v>148</v>
+      </c>
+      <c r="JY58" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="JZ58" t="n">
+        <v>103</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="3">
@@ -50960,8 +51308,14 @@
       <c r="JW59" s="2" t="n">
         <v>364</v>
       </c>
-      <c r="JX59" t="n">
+      <c r="JX59" s="2" t="n">
         <v>364</v>
+      </c>
+      <c r="JY59" s="2" t="n">
+        <v>320</v>
+      </c>
+      <c r="JZ59" t="n">
+        <v>320</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="3">
@@ -51816,8 +52170,14 @@
       <c r="JW60" s="2" t="n">
         <v>1.46</v>
       </c>
-      <c r="JX60" t="n">
+      <c r="JX60" s="2" t="n">
         <v>1.46</v>
+      </c>
+      <c r="JY60" s="2" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="JZ60" t="n">
+        <v>2.11</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="3">
@@ -52672,8 +53032,14 @@
       <c r="JW61" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="JX61" t="n">
+      <c r="JX61" s="2" t="n">
         <v>81</v>
+      </c>
+      <c r="JY61" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="JZ61" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="3">
@@ -53528,8 +53894,14 @@
       <c r="JW62" s="2" t="n">
         <v>64</v>
       </c>
-      <c r="JX62" t="n">
+      <c r="JX62" s="2" t="n">
         <v>64</v>
+      </c>
+      <c r="JY62" s="2" t="n">
+        <v>75</v>
+      </c>
+      <c r="JZ62" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="3">
@@ -54384,8 +54756,14 @@
       <c r="JW63" s="2" t="n">
         <v>42</v>
       </c>
-      <c r="JX63" t="n">
+      <c r="JX63" s="2" t="n">
         <v>42</v>
+      </c>
+      <c r="JY63" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="JZ63" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="3">
@@ -55240,8 +55618,14 @@
       <c r="JW64" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="JX64" t="n">
+      <c r="JX64" s="2" t="n">
         <v>24</v>
+      </c>
+      <c r="JY64" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="JZ64" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="3">
@@ -56096,8 +56480,14 @@
       <c r="JW65" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="JX65" t="n">
+      <c r="JX65" s="2" t="n">
         <v>19</v>
+      </c>
+      <c r="JY65" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="JZ65" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="3">
@@ -56952,8 +57342,14 @@
       <c r="JW66" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="JX66" t="n">
+      <c r="JX66" s="2" t="n">
         <v>9</v>
+      </c>
+      <c r="JY66" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JZ66" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="3">
@@ -57808,8 +58204,14 @@
       <c r="JW67" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JX67" t="n">
+      <c r="JX67" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="JY67" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JZ67" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="3">
@@ -58664,8 +59066,14 @@
       <c r="JW68" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="JX68" t="n">
+      <c r="JX68" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="JY68" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="JZ68" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="3">
@@ -59520,7 +59928,13 @@
       <c r="JW69" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="JX69" t="n">
+      <c r="JX69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JY69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="JZ69" t="n">
         <v>2</v>
       </c>
     </row>
@@ -60376,8 +60790,14 @@
       <c r="JW70" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="JX70" t="n">
+      <c r="JX70" s="2" t="n">
         <v>14</v>
+      </c>
+      <c r="JY70" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="JZ70" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="3">
@@ -61232,8 +61652,14 @@
       <c r="JW71" s="2" t="n">
         <v>64.3</v>
       </c>
-      <c r="JX71" t="n">
+      <c r="JX71" s="2" t="n">
         <v>64.3</v>
+      </c>
+      <c r="JY71" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="JZ71" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="3">
@@ -62088,8 +62514,14 @@
       <c r="JW72" s="2" t="n">
         <v>40.44</v>
       </c>
-      <c r="JX72" t="n">
+      <c r="JX72" s="2" t="n">
         <v>40.44</v>
+      </c>
+      <c r="JY72" s="2" t="n">
+        <v>22.86</v>
+      </c>
+      <c r="JZ72" t="n">
+        <v>22.86</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="3">
@@ -62944,8 +63376,14 @@
       <c r="JW73" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="JX73" t="n">
+      <c r="JX73" s="2" t="n">
         <v>26</v>
+      </c>
+      <c r="JY73" s="2" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="JZ73" t="n">
+        <v>12.8</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="3">
@@ -63800,8 +64238,14 @@
       <c r="JW74" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="JX74" t="n">
+      <c r="JX74" s="2" t="n">
         <v>33</v>
+      </c>
+      <c r="JY74" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JZ74" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="75" ht="13.8" customHeight="1" s="3">
@@ -64656,8 +65100,14 @@
       <c r="JW75" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="JX75" t="n">
+      <c r="JX75" s="2" t="n">
         <v>69</v>
+      </c>
+      <c r="JY75" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JZ75" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="3">
@@ -65512,8 +65962,14 @@
       <c r="JW76" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JX76" t="n">
+      <c r="JX76" s="2" t="n">
         <v>44</v>
+      </c>
+      <c r="JY76" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="JZ76" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="3">
@@ -66368,8 +66824,14 @@
       <c r="JW77" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="JX77" t="n">
+      <c r="JX77" s="2" t="n">
         <v>43</v>
+      </c>
+      <c r="JY77" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="JZ77" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="3">
@@ -67224,8 +67686,14 @@
       <c r="JW78" s="2" t="n">
         <v>3.07</v>
       </c>
-      <c r="JX78" t="n">
+      <c r="JX78" s="2" t="n">
         <v>3.07</v>
+      </c>
+      <c r="JY78" s="2" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="JZ78" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="3">
@@ -68080,8 +68548,14 @@
       <c r="JW79" s="2" t="n">
         <v>4.78</v>
       </c>
-      <c r="JX79" t="n">
+      <c r="JX79" s="2" t="n">
         <v>4.78</v>
+      </c>
+      <c r="JY79" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="JZ79" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="3">
@@ -68936,8 +69410,14 @@
       <c r="JW80" s="2" t="n">
         <v>27.9</v>
       </c>
-      <c r="JX80" t="n">
+      <c r="JX80" s="2" t="n">
         <v>27.9</v>
+      </c>
+      <c r="JY80" s="2" t="n">
+        <v>41.1</v>
+      </c>
+      <c r="JZ80" t="n">
+        <v>41.1</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="3">
@@ -69792,8 +70272,14 @@
       <c r="JW81" s="2" t="n">
         <v>20.9</v>
       </c>
-      <c r="JX81" t="n">
+      <c r="JX81" s="2" t="n">
         <v>20.9</v>
+      </c>
+      <c r="JY81" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="JZ81" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="3">
@@ -70648,8 +71134,14 @@
       <c r="JW82" s="2" t="n">
         <v>188.9</v>
       </c>
-      <c r="JX82" t="n">
+      <c r="JX82" s="2" t="n">
         <v>188.9</v>
+      </c>
+      <c r="JY82" s="2" t="n">
+        <v>187.5</v>
+      </c>
+      <c r="JZ82" t="n">
+        <v>187.5</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="3">
@@ -71504,8 +71996,14 @@
       <c r="JW83" s="2" t="n">
         <v>87.40000000000001</v>
       </c>
-      <c r="JX83" t="n">
+      <c r="JX83" s="2" t="n">
         <v>87.40000000000001</v>
+      </c>
+      <c r="JY83" s="2" t="n">
+        <v>85.8</v>
+      </c>
+      <c r="JZ83" t="n">
+        <v>85.8</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="3">
@@ -72360,8 +72858,14 @@
       <c r="JW84" s="2" t="n">
         <v>24.66</v>
       </c>
-      <c r="JX84" t="n">
+      <c r="JX84" s="2" t="n">
         <v>24.66</v>
+      </c>
+      <c r="JY84" s="2" t="n">
+        <v>25.66</v>
+      </c>
+      <c r="JZ84" t="n">
+        <v>25.66</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="3">
@@ -73216,8 +73720,14 @@
       <c r="JW85" s="2" t="n">
         <v>86.2</v>
       </c>
-      <c r="JX85" t="n">
+      <c r="JX85" s="2" t="n">
         <v>86.2</v>
+      </c>
+      <c r="JY85" s="2" t="n">
+        <v>114.7</v>
+      </c>
+      <c r="JZ85" t="n">
+        <v>114.7</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="3">
@@ -74072,8 +74582,14 @@
       <c r="JW86" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JX86" t="n">
+      <c r="JX86" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="JY86" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JZ86" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="3">
@@ -74928,8 +75444,14 @@
       <c r="JW87" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="JX87" t="n">
+      <c r="JX87" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="JY87" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="JZ87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="3">
@@ -75784,7 +76306,13 @@
       <c r="JW88" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="JX88" t="n">
+      <c r="JX88" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JY88" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JZ88" t="n">
         <v>5</v>
       </c>
     </row>
@@ -76640,8 +77168,14 @@
       <c r="JW89" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="JX89" t="n">
+      <c r="JX89" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="JY89" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JZ89" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="3">
@@ -77496,8 +78030,14 @@
       <c r="JW90" s="2" t="n">
         <v>151</v>
       </c>
-      <c r="JX90" t="n">
+      <c r="JX90" s="2" t="n">
         <v>151</v>
+      </c>
+      <c r="JY90" s="2" t="n">
+        <v>144</v>
+      </c>
+      <c r="JZ90" t="n">
+        <v>144</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="3">
@@ -78352,8 +78892,14 @@
       <c r="JW91" s="2" t="n">
         <v>206</v>
       </c>
-      <c r="JX91" t="n">
+      <c r="JX91" s="2" t="n">
         <v>206</v>
+      </c>
+      <c r="JY91" s="2" t="n">
+        <v>166</v>
+      </c>
+      <c r="JZ91" t="n">
+        <v>166</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="3">
@@ -79208,8 +79754,14 @@
       <c r="JW92" s="2" t="n">
         <v>266</v>
       </c>
-      <c r="JX92" t="n">
+      <c r="JX92" s="2" t="n">
         <v>266</v>
+      </c>
+      <c r="JY92" s="2" t="n">
+        <v>224</v>
+      </c>
+      <c r="JZ92" t="n">
+        <v>224</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="3">
@@ -80064,8 +80616,14 @@
       <c r="JW93" s="2" t="n">
         <v>73.09999999999999</v>
       </c>
-      <c r="JX93" t="n">
+      <c r="JX93" s="2" t="n">
         <v>73.09999999999999</v>
+      </c>
+      <c r="JY93" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="JZ93" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="3">
@@ -80920,8 +81478,14 @@
       <c r="JW94" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="JX94" t="n">
+      <c r="JX94" s="2" t="n">
         <v>69</v>
+      </c>
+      <c r="JY94" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="JZ94" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="3">
@@ -81776,8 +82340,14 @@
       <c r="JW95" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="JX95" t="n">
+      <c r="JX95" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="JY95" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="JZ95" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="3">
@@ -82632,8 +83202,14 @@
       <c r="JW96" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="JX96" t="n">
+      <c r="JX96" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="JY96" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="JZ96" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="3">
@@ -83488,8 +84064,14 @@
       <c r="JW97" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="JX97" t="n">
+      <c r="JX97" s="2" t="n">
         <v>33</v>
+      </c>
+      <c r="JY97" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="JZ97" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="98" ht="13.8" customHeight="1" s="3">
@@ -84344,8 +84926,14 @@
       <c r="JW98" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="JX98" t="n">
+      <c r="JX98" s="2" t="n">
         <v>44</v>
+      </c>
+      <c r="JY98" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="JZ98" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="3">
@@ -85200,8 +85788,14 @@
       <c r="JW99" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="JX99" t="n">
+      <c r="JX99" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="JY99" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="JZ99" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="3">
@@ -86056,8 +86650,14 @@
       <c r="JW100" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="JX100" t="n">
+      <c r="JX100" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="JY100" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="JZ100" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="101" ht="13.8" customHeight="1" s="3">
@@ -86912,8 +87512,14 @@
       <c r="JW101" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="JX101" t="n">
+      <c r="JX101" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="JY101" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="JZ101" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="3">
@@ -87768,8 +88374,14 @@
       <c r="JW102" s="2" t="n">
         <v>77.8</v>
       </c>
-      <c r="JX102" t="n">
+      <c r="JX102" s="2" t="n">
         <v>77.8</v>
+      </c>
+      <c r="JY102" s="2" t="n">
+        <v>42.9</v>
+      </c>
+      <c r="JZ102" t="n">
+        <v>42.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>